<commit_message>
ZSR-31  When DUT is in standby mode,BT connect,wake up DUT,Play BT audio,then connect AUX ZSR-30 Unknown situation crash,Did not enter standby mode for 10 minutes ZSR-32  When playing music, leaving the Bluetooth range, after 12 hours, the machine crashes, and there is no response when checking the power cord
</commit_message>
<xml_diff>
--- a/sw/project_files/Hendrix_M/Release/Hendrix_LiteV2_Notes/RD-Quick Test Report.xlsx
+++ b/sw/project_files/Hendrix_M/Release/Hendrix_LiteV2_Notes/RD-Quick Test Report.xlsx
@@ -12,14 +12,15 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7635" tabRatio="664"/>
   </bookViews>
   <sheets>
-    <sheet name="RDQT 6.0.3" sheetId="12" r:id="rId1"/>
-    <sheet name="RDQT 6.0.2" sheetId="11" r:id="rId2"/>
-    <sheet name="RDQT 1.0.2" sheetId="10" r:id="rId3"/>
-    <sheet name="RDQT 1.0.1" sheetId="9" r:id="rId4"/>
-    <sheet name="RDQT 1.0.0" sheetId="8" r:id="rId5"/>
+    <sheet name="RDQT 6.0.4" sheetId="13" r:id="rId1"/>
+    <sheet name="RDQT 6.0.3" sheetId="12" r:id="rId2"/>
+    <sheet name="RDQT 6.0.2" sheetId="11" r:id="rId3"/>
+    <sheet name="RDQT 1.0.2" sheetId="10" r:id="rId4"/>
+    <sheet name="RDQT 1.0.1" sheetId="9" r:id="rId5"/>
+    <sheet name="RDQT 1.0.0" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Light">[1]List!$A$2:$A$6</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="71">
   <si>
     <t>Pass</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -309,6 +310,12 @@
   </si>
   <si>
     <t>BT firmware havn't change</t>
+  </si>
+  <si>
+    <t>6.0.4</t>
+  </si>
+  <si>
+    <t>Hendrix_M_Lite_V2</t>
   </si>
 </sst>
 </file>
@@ -471,7 +478,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -504,6 +511,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -949,8 +959,8 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -965,14 +975,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="12" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -983,48 +993,48 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="33"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34">
-        <v>44392</v>
-      </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
+        <v>44396</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
@@ -1033,24 +1043,24 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
       <c r="A5" s="4">
@@ -1059,22 +1069,22 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
       <c r="A6" s="4">
@@ -1083,22 +1093,22 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="59.45" customHeight="1">
       <c r="A7" s="4">
@@ -1107,22 +1117,22 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="59.45" customHeight="1">
       <c r="A8" s="4">
@@ -1131,22 +1141,22 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="51" customHeight="1">
       <c r="A9" s="4">
@@ -1155,22 +1165,22 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="51" customHeight="1">
       <c r="A10" s="4">
@@ -1179,22 +1189,22 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" ht="52.15" customHeight="1">
       <c r="A11" s="4">
@@ -1203,24 +1213,24 @@
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="49.9" customHeight="1">
       <c r="A12" s="4">
@@ -1229,22 +1239,22 @@
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="70.900000000000006" customHeight="1">
       <c r="A13" s="4">
@@ -1253,22 +1263,22 @@
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="59.45" customHeight="1">
       <c r="A14" s="4">
@@ -1277,22 +1287,22 @@
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="59.45" customHeight="1">
       <c r="A15" s="10">
@@ -1301,18 +1311,18 @@
       <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="59.45" customHeight="1">
       <c r="A16" s="10">
@@ -1321,18 +1331,18 @@
       <c r="B16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" ht="59.45" customHeight="1">
       <c r="A17" s="10">
@@ -1341,18 +1351,18 @@
       <c r="B17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="4"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" ht="59.45" customHeight="1">
       <c r="A18" s="10">
@@ -1361,18 +1371,18 @@
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="4"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="59.45" customHeight="1">
       <c r="A19" s="4">
@@ -1381,36 +1391,36 @@
       <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" ht="59.45" customHeight="1">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -1471,7 +1481,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+      <selection activeCell="J9" sqref="J9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1486,14 +1496,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="11" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -1504,48 +1514,48 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="33"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34">
-        <v>44361</v>
-      </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
+        <v>44392</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
@@ -1554,24 +1564,24 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
       <c r="A5" s="4">
@@ -1580,22 +1590,22 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
       <c r="A6" s="4">
@@ -1604,22 +1614,22 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="59.45" customHeight="1">
       <c r="A7" s="4">
@@ -1628,22 +1638,22 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="59.45" customHeight="1">
       <c r="A8" s="4">
@@ -1652,22 +1662,22 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="51" customHeight="1">
       <c r="A9" s="4">
@@ -1676,22 +1686,22 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="51" customHeight="1">
       <c r="A10" s="4">
@@ -1700,22 +1710,22 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" ht="52.15" customHeight="1">
       <c r="A11" s="4">
@@ -1724,22 +1734,24 @@
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
+        <v>67</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="49.9" customHeight="1">
       <c r="A12" s="4">
@@ -1748,22 +1760,22 @@
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="70.900000000000006" customHeight="1">
       <c r="A13" s="4">
@@ -1772,22 +1784,22 @@
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="59.45" customHeight="1">
       <c r="A14" s="4">
@@ -1796,22 +1808,22 @@
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4" t="s">
         <v>64</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="59.45" customHeight="1">
       <c r="A15" s="10">
@@ -1820,18 +1832,18 @@
       <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="59.45" customHeight="1">
       <c r="A16" s="10">
@@ -1840,18 +1852,18 @@
       <c r="B16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" ht="59.45" customHeight="1">
       <c r="A17" s="10">
@@ -1860,18 +1872,18 @@
       <c r="B17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="4"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" ht="59.45" customHeight="1">
       <c r="A18" s="10">
@@ -1880,18 +1892,18 @@
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="4"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="59.45" customHeight="1">
       <c r="A19" s="4">
@@ -1900,36 +1912,36 @@
       <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" ht="59.45" customHeight="1">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
       <c r="H20" s="4"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -1990,7 +2002,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:G7"/>
+      <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -2005,14 +2017,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="8" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -2023,48 +2035,48 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="33"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34">
-        <v>43654</v>
-      </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
+        <v>44361</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
@@ -2073,24 +2085,24 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
       <c r="A5" s="4">
@@ -2099,22 +2111,22 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
       <c r="A6" s="4">
@@ -2123,22 +2135,22 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="59.45" customHeight="1">
       <c r="A7" s="4">
@@ -2147,22 +2159,22 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="59.45" customHeight="1">
       <c r="A8" s="4">
@@ -2171,22 +2183,22 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="51" customHeight="1">
       <c r="A9" s="4">
@@ -2195,22 +2207,22 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="51" customHeight="1">
       <c r="A10" s="4">
@@ -2219,22 +2231,22 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" ht="52.15" customHeight="1">
       <c r="A11" s="4">
@@ -2243,22 +2255,22 @@
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="49.9" customHeight="1">
       <c r="A12" s="4">
@@ -2267,22 +2279,22 @@
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="70.900000000000006" customHeight="1">
       <c r="A13" s="4">
@@ -2291,22 +2303,22 @@
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="59.45" customHeight="1">
       <c r="A14" s="4">
@@ -2315,22 +2327,22 @@
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="59.45" customHeight="1">
       <c r="A15" s="10">
@@ -2339,22 +2351,18 @@
       <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="59.45" customHeight="1">
       <c r="A16" s="10">
@@ -2363,22 +2371,18 @@
       <c r="B16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" ht="59.45" customHeight="1">
       <c r="A17" s="10">
@@ -2387,22 +2391,18 @@
       <c r="B17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" ht="59.45" customHeight="1">
       <c r="A18" s="10">
@@ -2411,22 +2411,18 @@
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="59.45" customHeight="1">
       <c r="A19" s="4">
@@ -2435,40 +2431,36 @@
       <c r="B19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
     </row>
     <row r="20" spans="1:12" ht="59.45" customHeight="1">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="4"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="43">
@@ -2516,13 +2508,552 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:L2"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="8.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="2" customWidth="1"/>
+    <col min="3" max="7" width="9" style="2"/>
+    <col min="8" max="8" width="11.375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9" style="2"/>
+    <col min="12" max="12" width="51" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
+        <v>43654</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
+    </row>
+    <row r="6" spans="1:12" ht="40.9" customHeight="1">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
+    </row>
+    <row r="7" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A7" s="4">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A8" s="4">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" ht="51" customHeight="1">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" ht="51" customHeight="1">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" ht="52.15" customHeight="1">
+      <c r="A11" s="4">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
+    </row>
+    <row r="12" spans="1:12" ht="49.9" customHeight="1">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
+    </row>
+    <row r="13" spans="1:12" ht="70.900000000000006" customHeight="1">
+      <c r="A13" s="4">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A14" s="4">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A15" s="10">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A16" s="10">
+        <v>12</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A17" s="10">
+        <v>13</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A18" s="10">
+        <v>14</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A19" s="4">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" ht="59.45" customHeight="1">
+      <c r="A20" s="4">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="43">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="J18:L18"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2545,13 +3076,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
@@ -2563,48 +3094,48 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="33"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34">
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
         <v>43189</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
@@ -2613,24 +3144,24 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
       <c r="A5" s="4">
@@ -2639,22 +3170,22 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
       <c r="A6" s="4">
@@ -2663,22 +3194,22 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="59.45" customHeight="1">
       <c r="A7" s="4">
@@ -2687,22 +3218,22 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="59.45" customHeight="1">
       <c r="A8" s="4">
@@ -2711,22 +3242,22 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="51" customHeight="1">
       <c r="A9" s="4">
@@ -2735,22 +3266,22 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="51" customHeight="1">
       <c r="A10" s="4">
@@ -2759,22 +3290,22 @@
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" spans="1:12" ht="52.15" customHeight="1">
       <c r="A11" s="4">
@@ -2783,22 +3314,22 @@
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="1:12" ht="49.9" customHeight="1">
       <c r="A12" s="4">
@@ -2807,22 +3338,22 @@
       <c r="B12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="70.900000000000006" customHeight="1">
       <c r="A13" s="4">
@@ -2831,22 +3362,22 @@
       <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="15"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="59.45" customHeight="1">
       <c r="A14" s="4">
@@ -2855,22 +3386,22 @@
       <c r="B14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="59.45" customHeight="1">
       <c r="A15" s="4">
@@ -2879,22 +3410,22 @@
       <c r="B15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="15"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16" spans="1:12" ht="59.45" customHeight="1">
       <c r="A16" s="4">
@@ -2903,22 +3434,22 @@
       <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="15"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
     </row>
     <row r="17" spans="1:12" ht="59.45" customHeight="1">
       <c r="A17" s="4">
@@ -2927,22 +3458,22 @@
       <c r="B17" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
       <c r="H17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="15"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="1:12" ht="59.45" customHeight="1">
       <c r="A18" s="4">
@@ -2951,57 +3482,28 @@
       <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="J18" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="K18" s="14"/>
-      <c r="L18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
     </row>
     <row r="19" spans="1:12" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="J11:L11"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="J17:L17"/>
     <mergeCell ref="C18:G18"/>
@@ -3012,6 +3514,35 @@
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:L2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3019,7 +3550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -3040,13 +3571,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3058,48 +3589,48 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30" t="s">
+      <c r="D2" s="30"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="32"/>
+      <c r="H2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="33"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="30" t="s">
+      <c r="D3" s="30"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="34">
+      <c r="G3" s="32"/>
+      <c r="H3" s="35">
         <v>43041</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="3" t="s">
@@ -3108,24 +3639,24 @@
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:12" ht="67.900000000000006" customHeight="1">
       <c r="A5" s="4">
@@ -3134,24 +3665,24 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" spans="1:12" ht="40.9" customHeight="1">
       <c r="A6" s="4">
@@ -3160,22 +3691,22 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
     </row>
     <row r="7" spans="1:12" ht="59.45" customHeight="1">
       <c r="A7" s="4">
@@ -3184,22 +3715,22 @@
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="1:12" ht="59.45" customHeight="1">
       <c r="A8" s="4">
@@ -3208,22 +3739,22 @@
       <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="15"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
     </row>
     <row r="9" spans="1:12" ht="51" customHeight="1">
       <c r="A9" s="4">
@@ -3232,24 +3763,24 @@
       <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" ht="59.45" customHeight="1">
       <c r="A10" s="4">
@@ -3258,22 +3789,22 @@
       <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
       <c r="H10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="15"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:12" ht="51" customHeight="1">
       <c r="A11" s="4">
@@ -3282,24 +3813,24 @@
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="14"/>
-      <c r="L11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12" ht="52.15" customHeight="1">
       <c r="A12" s="4">
@@ -3308,54 +3839,54 @@
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="23"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="24"/>
     </row>
     <row r="13" spans="1:12" ht="49.9" customHeight="1">
       <c r="A13" s="4">
         <v>9</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="23"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" ht="70.900000000000006" customHeight="1">
       <c r="A14" s="4">
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="15"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
     </row>
     <row r="15" spans="1:12" ht="59.45" customHeight="1"/>
     <row r="16" spans="1:12" ht="59.45" customHeight="1"/>
@@ -3365,28 +3896,6 @@
     <row r="20" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:G3"/>
@@ -3396,6 +3905,28 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:L2"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="J12:L12"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3403,6 +3934,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="72de59d5-254d-430a-8862-e2bf58cab753">6TCUH2D2FU37-209-14453</_dlc_DocId>
@@ -3414,66 +3954,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006ADE9B120D8C2544A30794E0CE6B3CF6" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6b7a23d33ee8a228344a1c6303b6d86b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="72de59d5-254d-430a-8862-e2bf58cab753" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b905d02d852158c2afe173951ebabb5b" ns2:_="">
     <xsd:import namespace="72de59d5-254d-430a-8862-e2bf58cab753"/>
@@ -3618,7 +4099,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0AA1759-4A2E-4491-9C5A-7766559224EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90A17C51-7000-43B7-9373-E2C13FAD8445}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -3634,23 +4173,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0AA1759-4A2E-4491-9C5A-7766559224EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFF19337-409A-4CFF-80EA-D2526D7612D6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6290CC7F-B9B0-4D98-A55D-A30816CE8732}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3666,4 +4189,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFF19337-409A-4CFF-80EA-D2526D7612D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>